<commit_message>
added appconfig and STATE MANAGEMENT IS WORKING
</commit_message>
<xml_diff>
--- a/SeedingResources/ApplicationConfiguration.xlsx
+++ b/SeedingResources/ApplicationConfiguration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\CyberMuffin\Repos\BlazorEcommerce\SeedingResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49194F88-9301-499A-9AE6-A62B876AE9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A88A9A-6DF4-45CB-AFAE-92F8A6F0A024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3675" yWindow="3675" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,12 +366,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>

</xml_diff>